<commit_message>
Completed Working with Excel Name Ranges
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57de5c48f32aaca3/OfficeNewb/Videos/MicrosoftOffice/Excel103/Exercise Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1467" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0001BDCB-2EA0-4C8E-8B79-3D4FCD1A5087}"/>
+  <xr:revisionPtr revIDLastSave="1476" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBE5BD6F-5D84-4168-88D7-425BE394E8F1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -98,6 +98,10 @@
     <definedName name="solver_val" localSheetId="15" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="15" hidden="1">3</definedName>
+    <definedName name="Week_1">'IF Function'!$B$5:$B$9</definedName>
+    <definedName name="Week_2">'IF Function'!$C$5:$C$9</definedName>
+    <definedName name="Week_3">'IF Function'!$D$5:$D$9</definedName>
+    <definedName name="Week_4">'IF Function'!$E$5:$E$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -972,15 +976,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
-    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00;\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1617,20 +1620,20 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1639,7 +1642,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1648,29 +1651,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1683,19 +1686,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1704,7 +1707,7 @@
     <xf numFmtId="37" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="5" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1731,16 +1734,16 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1758,7 +1761,7 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1766,21 +1769,19 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1811,20 +1812,20 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1832,18 +1833,18 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="10" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1853,23 +1854,23 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="9" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="9" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="9" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="9" borderId="3" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="9" borderId="27" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="9" borderId="27" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="28" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1881,7 +1882,7 @@
     <xf numFmtId="1" fontId="17" fillId="8" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="8" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="17" fillId="8" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1897,37 +1898,37 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="29" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="11" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="3" fillId="11" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="11" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="11" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="11" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="11" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="11" borderId="3" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="7" fillId="11" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="11" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="9" borderId="3" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1944,7 +1945,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1965,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2670,33 +2671,33 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="1.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="129" t="s">
+    <row r="1" spans="1:9" ht="13" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
+      <c r="A2" s="127" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2704,8 +2705,8 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="4" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="13.5" thickTop="1" thickBot="1"/>
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -2727,11 +2728,11 @@
       <c r="H4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2754,7 +2755,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2777,7 +2778,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2800,7 +2801,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -2823,50 +2824,62 @@
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="50">
         <v>7892</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="50">
         <v>7695</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="50">
         <v>9520</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="50">
         <v>10252</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="51">
         <f>SUM(B9:E9)</f>
         <v>35359</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-    </row>
-    <row r="11" spans="1:9" s="50" customFormat="1" ht="15">
+      <c r="B10" s="53">
+        <f>SUM(Week_1)</f>
+        <v>40402</v>
+      </c>
+      <c r="C10" s="53">
+        <f>SUM(Week_2)</f>
+        <v>42555</v>
+      </c>
+      <c r="D10" s="53">
+        <f>SUM(Week_3)</f>
+        <v>46630</v>
+      </c>
+      <c r="E10" s="53">
+        <f>SUM(Week_4)</f>
+        <v>46624</v>
+      </c>
+      <c r="F10" s="53"/>
+    </row>
+    <row r="11" spans="1:9" ht="14">
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="126" t="s">
+      <c r="A12" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="127"/>
-      <c r="C12" s="127"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="128"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
       <c r="F12" s="3"/>
     </row>
   </sheetData>
@@ -2890,21 +2903,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:3" ht="15.5">
+      <c r="A1" s="70" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="70" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2948,191 +2961,198 @@
       <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="3.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" ht="13">
       <c r="B2" s="40" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="134" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="134"/>
-    </row>
-    <row r="3" spans="2:6">
+      <c r="F2" s="130"/>
+    </row>
+    <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="132" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="133"/>
-    </row>
-    <row r="4" spans="2:6">
+      <c r="F3" s="132"/>
+    </row>
+    <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="132"/>
-      <c r="F4" s="133"/>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
+    </row>
+    <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="132"/>
-      <c r="F5" s="133"/>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
+    </row>
+    <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="132"/>
-      <c r="F6" s="133"/>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
+    </row>
+    <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="132"/>
-      <c r="F7" s="133"/>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
+    </row>
+    <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="132"/>
-      <c r="F8" s="133"/>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
+    </row>
+    <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="132"/>
-      <c r="F9" s="133"/>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
+    </row>
+    <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="132"/>
-      <c r="F10" s="133"/>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
+    </row>
+    <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="132"/>
-      <c r="F11" s="133"/>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
+    </row>
+    <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="132"/>
-      <c r="F12" s="133"/>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
+    </row>
+    <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="132"/>
-      <c r="F13" s="133"/>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
+    </row>
+    <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="132"/>
-      <c r="F14" s="133"/>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
+    </row>
+    <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="132"/>
-      <c r="F15" s="133"/>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
+    </row>
+    <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="132"/>
-      <c r="F16" s="133"/>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
+    </row>
+    <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="132"/>
-      <c r="F17" s="133"/>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
+    </row>
+    <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
         <v>77</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="132"/>
-      <c r="F18" s="133"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3143,13 +3163,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3166,29 +3179,29 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="1.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="129" t="s">
+    <row r="1" spans="1:9" ht="13" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
+      <c r="A2" s="127" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3196,8 +3209,8 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="4" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="13.5" thickTop="1" thickBot="1"/>
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -3219,11 +3232,11 @@
       <c r="H4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -3252,7 +3265,7 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -3281,7 +3294,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -3310,7 +3323,7 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3339,23 +3352,23 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="51">
+      <c r="B9" s="50">
         <v>7892</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="50">
         <v>7695</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="50">
         <v>9520</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="50">
         <v>10252</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="51">
         <f>SUM(B9:E9)</f>
         <v>35359</v>
       </c>
@@ -3368,32 +3381,32 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="53">
         <f>SUM(B5:B9)</f>
         <v>40402</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="53">
         <f t="shared" ref="C10:F10" si="2">SUM(C5:C9)</f>
         <v>42555</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="53">
         <f t="shared" si="2"/>
         <v>46630</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="53">
         <f t="shared" si="2"/>
         <v>46624</v>
       </c>
-      <c r="F10" s="54">
+      <c r="F10" s="53">
         <f t="shared" si="2"/>
         <v>176211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="50" customFormat="1" ht="15">
+    <row r="11" spans="1:9" ht="14">
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
@@ -3407,13 +3420,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="127"/>
-      <c r="C14" s="127"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="128"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -3439,14 +3452,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
-      <c r="A2" s="71" t="s">
+    <row r="2" spans="1:2" ht="13">
+      <c r="A2" s="69" t="s">
         <v>249</v>
       </c>
       <c r="B2" s="9">
@@ -3468,29 +3481,29 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="1.1796875" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" thickBot="1"/>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A2" s="129" t="s">
+    <row r="1" spans="1:9" ht="13" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
+      <c r="A2" s="127" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3498,8 +3511,8 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25" thickTop="1" thickBot="1"/>
-    <row r="4" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="13.5" thickTop="1" thickBot="1"/>
+    <row r="4" spans="1:9" ht="14">
       <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
@@ -3521,24 +3534,24 @@
       <c r="H4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="73">
+      <c r="B5" s="71">
         <v>9550</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="71">
         <v>9230</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="71">
         <v>8500</v>
       </c>
-      <c r="E5" s="73">
+      <c r="E5" s="71">
         <v>8965</v>
       </c>
       <c r="F5" s="15">
@@ -3554,20 +3567,20 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75">
+    <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="71">
         <v>5975</v>
       </c>
-      <c r="C6" s="73">
+      <c r="C6" s="71">
         <v>6900</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="71">
         <v>8500</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="71">
         <v>10100</v>
       </c>
       <c r="F6" s="15">
@@ -3583,20 +3596,20 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75">
+    <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="71">
         <v>7425</v>
       </c>
-      <c r="C7" s="73">
+      <c r="C7" s="71">
         <v>8580</v>
       </c>
-      <c r="D7" s="73">
+      <c r="D7" s="71">
         <v>9910</v>
       </c>
-      <c r="E7" s="73">
+      <c r="E7" s="71">
         <v>7512</v>
       </c>
       <c r="F7" s="15">
@@ -3612,20 +3625,20 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75">
+    <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="73">
+      <c r="B8" s="71">
         <v>9560</v>
       </c>
-      <c r="C8" s="73">
+      <c r="C8" s="71">
         <v>10150</v>
       </c>
-      <c r="D8" s="73">
+      <c r="D8" s="71">
         <v>10200</v>
       </c>
-      <c r="E8" s="73">
+      <c r="E8" s="71">
         <v>9795</v>
       </c>
       <c r="F8" s="15">
@@ -3641,23 +3654,23 @@
         <v>BONUS</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1">
+    <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="74">
+      <c r="B9" s="72">
         <v>7892</v>
       </c>
-      <c r="C9" s="74">
+      <c r="C9" s="72">
         <v>7695</v>
       </c>
-      <c r="D9" s="74">
+      <c r="D9" s="72">
         <v>9520</v>
       </c>
-      <c r="E9" s="74">
+      <c r="E9" s="72">
         <v>10252</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="51">
         <f>SUM(B9:E9)</f>
         <v>35359</v>
       </c>
@@ -3670,32 +3683,32 @@
         <v>NO BONUS</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="53">
         <f>SUM(B5:B9)</f>
         <v>40402</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="53">
         <f t="shared" ref="C10:F10" si="2">SUM(C5:C9)</f>
         <v>42555</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="53">
         <f t="shared" si="2"/>
         <v>46630</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="53">
         <f t="shared" si="2"/>
         <v>46624</v>
       </c>
-      <c r="F10" s="54">
+      <c r="F10" s="53">
         <f t="shared" si="2"/>
         <v>176211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="50" customFormat="1" ht="15">
+    <row r="11" spans="1:9" ht="14">
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
@@ -3710,13 +3723,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="126" t="s">
+      <c r="A14" s="124" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="127"/>
-      <c r="C14" s="127"/>
-      <c r="D14" s="127"/>
-      <c r="E14" s="128"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -3742,45 +3755,45 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.5" thickBot="1"/>
-    <row r="2" spans="1:4">
-      <c r="A2" s="98" t="s">
+    <row r="1" spans="1:4" ht="13" thickBot="1"/>
+    <row r="2" spans="1:4" ht="13">
+      <c r="A2" s="96" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="93">
+      <c r="B2" s="91">
         <v>220000</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="97" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="95" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="96" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="94">
+      <c r="B3" s="92">
         <v>0.08</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="96"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="98" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="94"/>
+    </row>
+    <row r="4" spans="1:4" ht="13">
+      <c r="A4" s="96" t="s">
         <v>251</v>
       </c>
-      <c r="B4" s="95">
+      <c r="B4" s="93">
         <v>300</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3796,192 +3809,192 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="79" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="79" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="79" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="79" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="79" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="79" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="79" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="79" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="79"/>
+    <col min="1" max="1" width="25.453125" style="77" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="77" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" style="77" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="77" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="77" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" style="77" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" style="77" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" style="77" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="10.5" customHeight="1">
-      <c r="A1" s="92"/>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="A1" s="90"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
     </row>
     <row r="2" spans="1:8" ht="11.25" customHeight="1" thickBot="1"/>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="G3" s="102" t="s">
+      <c r="G3" s="100" t="s">
         <v>272</v>
       </c>
-      <c r="H3" s="103" t="s">
+      <c r="H3" s="101" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" thickBot="1">
-      <c r="A4" s="90" t="s">
+    <row r="4" spans="1:8" ht="16" thickBot="1">
+      <c r="A4" s="88" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="99" t="s">
         <v>276</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="99" t="s">
         <v>275</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="99" t="s">
         <v>274</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="104" t="s">
+      <c r="F4" s="73"/>
+      <c r="G4" s="102" t="s">
         <v>273</v>
       </c>
-      <c r="H4" s="105" t="s">
+      <c r="H4" s="103" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
-      <c r="A5" s="88" t="s">
+    <row r="5" spans="1:8" ht="15.5">
+      <c r="A5" s="86" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="87">
+      <c r="B5" s="85">
         <v>1</v>
       </c>
-      <c r="C5" s="87">
+      <c r="C5" s="85">
         <v>1</v>
       </c>
-      <c r="D5" s="87">
+      <c r="D5" s="85">
         <v>1</v>
       </c>
-      <c r="E5" s="87">
+      <c r="E5" s="85">
         <v>1</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="86">
+      <c r="F5" s="73"/>
+      <c r="G5" s="84">
         <v>1.25</v>
       </c>
-      <c r="H5" s="85">
+      <c r="H5" s="83">
         <f>G5*(B5+C5+D5+E5)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
-      <c r="A6" s="88" t="s">
+    <row r="6" spans="1:8" ht="15.5">
+      <c r="A6" s="86" t="s">
         <v>270</v>
       </c>
-      <c r="B6" s="89">
+      <c r="B6" s="87">
         <v>0</v>
       </c>
-      <c r="C6" s="87">
+      <c r="C6" s="85">
         <v>0</v>
       </c>
-      <c r="D6" s="87">
+      <c r="D6" s="85">
         <v>0</v>
       </c>
-      <c r="E6" s="87">
+      <c r="E6" s="85">
         <v>0</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="86">
+      <c r="F6" s="73"/>
+      <c r="G6" s="84">
         <v>1.84</v>
       </c>
-      <c r="H6" s="85">
+      <c r="H6" s="83">
         <f>G6*(B6+C6+D6+E6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
-      <c r="A7" s="88" t="s">
+    <row r="7" spans="1:8" ht="15.5">
+      <c r="A7" s="86" t="s">
         <v>269</v>
       </c>
-      <c r="B7" s="87">
+      <c r="B7" s="85">
         <v>0</v>
       </c>
-      <c r="C7" s="87">
+      <c r="C7" s="85">
         <v>0</v>
       </c>
-      <c r="D7" s="87">
+      <c r="D7" s="85">
         <v>0</v>
       </c>
-      <c r="E7" s="87">
+      <c r="E7" s="85">
         <v>0</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="86">
+      <c r="F7" s="73"/>
+      <c r="G7" s="84">
         <v>1.45</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="83">
         <f>G7*(B7+C7+D7+E7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
-      <c r="A8" s="99" t="s">
+    <row r="8" spans="1:8" ht="15.5">
+      <c r="A8" s="97" t="s">
         <v>268</v>
       </c>
-      <c r="B8" s="84">
+      <c r="B8" s="82">
         <f>SUM(B5:B7)</f>
         <v>1</v>
       </c>
-      <c r="C8" s="84">
+      <c r="C8" s="82">
         <f>SUM(C5:C7)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="84">
+      <c r="D8" s="82">
         <f>SUM(D5:D7)</f>
         <v>1</v>
       </c>
-      <c r="E8" s="84">
+      <c r="E8" s="82">
         <f>SUM(E5:E7)</f>
         <v>1</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="106">
+      <c r="F8" s="73"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="104">
         <f>H5+H6+H7</f>
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="4.5" customHeight="1">
-      <c r="A9" s="82"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="75"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75">
-      <c r="A10" s="100" t="s">
+      <c r="A9" s="80"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="73"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.5">
+      <c r="A10" s="98" t="s">
         <v>267</v>
       </c>
-      <c r="B10" s="107">
+      <c r="B10" s="105">
         <v>180</v>
       </c>
-      <c r="C10" s="107">
+      <c r="C10" s="105">
         <v>80</v>
       </c>
-      <c r="D10" s="107">
+      <c r="D10" s="105">
         <v>190</v>
       </c>
-      <c r="E10" s="107">
+      <c r="E10" s="105">
         <v>160</v>
       </c>
-      <c r="F10" s="75"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75">
-      <c r="A11" s="80"/>
-      <c r="F11" s="75"/>
+      <c r="F10" s="73"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.5">
+      <c r="A11" s="78"/>
+      <c r="F11" s="73"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" gridLinesSet="0"/>
@@ -4004,89 +4017,89 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="75"/>
-    <col min="2" max="2" width="17.42578125" style="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.42578125" style="75" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="75"/>
+    <col min="1" max="1" width="9.1796875" style="73"/>
+    <col min="2" max="2" width="17.453125" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="12.453125" style="73" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="73"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="98" t="s">
+    <row r="2" spans="2:3" ht="13">
+      <c r="B2" s="96" t="s">
         <v>254</v>
       </c>
-      <c r="C2" s="108">
+      <c r="C2" s="106">
         <v>220000</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="98" t="s">
+    <row r="3" spans="2:3" ht="13">
+      <c r="B3" s="96" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="109">
+      <c r="C3" s="107">
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="98" t="s">
+    <row r="4" spans="2:3" ht="13">
+      <c r="B4" s="96" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="110">
+      <c r="C4" s="108">
         <f>25*12</f>
         <v>300</v>
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="C6" s="77"/>
-    </row>
-    <row r="7" spans="2:3" ht="15.75">
-      <c r="B7" s="112" t="s">
+      <c r="C6" s="75"/>
+    </row>
+    <row r="7" spans="2:3" ht="15.5">
+      <c r="B7" s="110" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="111">
+      <c r="C7" s="109">
         <f>-PMT(C3/12,C4,C2)</f>
         <v>1697.9956826206067</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75">
-      <c r="B8" s="76">
+    <row r="8" spans="2:3" ht="15.5">
+      <c r="B8" s="74">
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75">
-      <c r="B9" s="76">
+    <row r="9" spans="2:3" ht="15.5">
+      <c r="B9" s="74">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="2:3" ht="15.75">
-      <c r="B10" s="76">
+    <row r="10" spans="2:3" ht="15.5">
+      <c r="B10" s="74">
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="C10" s="12"/>
     </row>
-    <row r="11" spans="2:3" ht="15.75">
-      <c r="B11" s="76">
+    <row r="11" spans="2:3" ht="15.5">
+      <c r="B11" s="74">
         <v>8.2500000000000004E-2</v>
       </c>
       <c r="C11" s="12"/>
     </row>
-    <row r="12" spans="2:3" ht="15.75">
-      <c r="B12" s="76">
+    <row r="12" spans="2:3" ht="15.5">
+      <c r="B12" s="74">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="C12" s="12"/>
     </row>
-    <row r="13" spans="2:3" ht="15.75">
-      <c r="B13" s="76">
+    <row r="13" spans="2:3" ht="15.5">
+      <c r="B13" s="74">
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C13" s="12"/>
     </row>
-    <row r="14" spans="2:3" ht="15.75">
-      <c r="B14" s="76">
+    <row r="14" spans="2:3" ht="15.5">
+      <c r="B14" s="74">
         <v>0.09</v>
       </c>
       <c r="C14" s="12"/>
@@ -4111,191 +4124,191 @@
       <selection activeCell="C11" sqref="C11:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="75"/>
-    <col min="2" max="2" width="11.5703125" style="75" customWidth="1"/>
-    <col min="3" max="6" width="14.85546875" style="75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="75" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="75"/>
+    <col min="1" max="1" width="9.1796875" style="73"/>
+    <col min="2" max="2" width="11.54296875" style="73" customWidth="1"/>
+    <col min="3" max="6" width="14.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="73"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75">
-      <c r="B2" s="112" t="s">
+    <row r="2" spans="2:7" ht="15.5">
+      <c r="B2" s="110" t="s">
         <v>266</v>
       </c>
-      <c r="C2" s="112" t="s">
+      <c r="C2" s="110" t="s">
         <v>265</v>
       </c>
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="110" t="s">
         <v>264</v>
       </c>
-      <c r="E2" s="112" t="s">
+      <c r="E2" s="110" t="s">
         <v>263</v>
       </c>
-      <c r="F2" s="112" t="s">
+      <c r="F2" s="110" t="s">
         <v>262</v>
       </c>
-      <c r="G2" s="112" t="s">
+      <c r="G2" s="110" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="113" t="s">
+    <row r="3" spans="2:7" ht="13">
+      <c r="B3" s="111" t="s">
         <v>258</v>
       </c>
-      <c r="C3" s="114">
+      <c r="C3" s="112">
         <v>85292.25</v>
       </c>
-      <c r="D3" s="114">
+      <c r="D3" s="112">
         <f>C3*C11+C3</f>
         <v>88106.894249999998</v>
       </c>
-      <c r="E3" s="114">
+      <c r="E3" s="112">
         <f>D3*C11+D3</f>
         <v>91014.421760249999</v>
       </c>
-      <c r="F3" s="114">
+      <c r="F3" s="112">
         <f>E3*C11+E3</f>
         <v>94017.897678338253</v>
       </c>
-      <c r="G3" s="114">
+      <c r="G3" s="112">
         <f>SUM(C3:F3)</f>
         <v>358431.46368858824</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="113" t="s">
+    <row r="4" spans="2:7" ht="13">
+      <c r="B4" s="111" t="s">
         <v>257</v>
       </c>
-      <c r="C4" s="114">
+      <c r="C4" s="112">
         <v>75891.25</v>
       </c>
-      <c r="D4" s="114">
+      <c r="D4" s="112">
         <f>C4*C12+C4</f>
         <v>77636.748749999999</v>
       </c>
-      <c r="E4" s="114">
+      <c r="E4" s="112">
         <f>D4*C12+D4</f>
         <v>79422.39397125</v>
       </c>
-      <c r="F4" s="114">
+      <c r="F4" s="112">
         <f>E4*C12+E4</f>
         <v>81249.109032588749</v>
       </c>
-      <c r="G4" s="114">
+      <c r="G4" s="112">
         <f>SUM(C4:F4)</f>
         <v>314199.50175383873</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="113" t="s">
+    <row r="5" spans="2:7" ht="13">
+      <c r="B5" s="111" t="s">
         <v>256</v>
       </c>
-      <c r="C5" s="114">
+      <c r="C5" s="112">
         <v>90568.34</v>
       </c>
-      <c r="D5" s="114">
+      <c r="D5" s="112">
         <f>C5*C13+C5</f>
         <v>94462.778619999997</v>
       </c>
-      <c r="E5" s="114">
+      <c r="E5" s="112">
         <f>D5*C13+D5</f>
         <v>98524.678100659992</v>
       </c>
-      <c r="F5" s="114">
+      <c r="F5" s="112">
         <f>E5*C13+E5</f>
         <v>102761.23925898837</v>
       </c>
-      <c r="G5" s="114">
+      <c r="G5" s="112">
         <f>SUM(C5:F5)</f>
         <v>386317.03597964835</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="113" t="s">
+    <row r="6" spans="2:7" ht="13">
+      <c r="B6" s="111" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="114">
+      <c r="C6" s="112">
         <v>65897.25</v>
       </c>
-      <c r="D6" s="114">
+      <c r="D6" s="112">
         <f>C6*C14+C6</f>
         <v>66622.119749999998</v>
       </c>
-      <c r="E6" s="114">
+      <c r="E6" s="112">
         <f>D6*C14+D6</f>
         <v>67354.963067249992</v>
       </c>
-      <c r="F6" s="114">
+      <c r="F6" s="112">
         <f>E6*C14+E6</f>
         <v>68095.867660989737</v>
       </c>
-      <c r="G6" s="114">
+      <c r="G6" s="112">
         <f>SUM(C6:F6)</f>
         <v>267970.20047823974</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75">
-      <c r="B7" s="101" t="s">
+    <row r="7" spans="2:7" ht="15.5">
+      <c r="B7" s="99" t="s">
         <v>260</v>
       </c>
-      <c r="C7" s="78">
+      <c r="C7" s="76">
         <f>SUM(C3:C6)</f>
         <v>317649.08999999997</v>
       </c>
-      <c r="D7" s="78">
+      <c r="D7" s="76">
         <f>SUM(D3:D6)</f>
         <v>326828.54136999999</v>
       </c>
-      <c r="E7" s="78">
+      <c r="E7" s="76">
         <f>SUM(E3:E6)</f>
         <v>336316.45689940994</v>
       </c>
-      <c r="F7" s="78">
+      <c r="F7" s="76">
         <f>SUM(F3:F6)</f>
         <v>346124.11363090511</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="76">
         <f>SUM(G3:G6)</f>
         <v>1326918.201900315</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="135" t="s">
+    <row r="10" spans="2:7" ht="13">
+      <c r="B10" s="133" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="135"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="115" t="s">
+      <c r="C10" s="133"/>
+    </row>
+    <row r="11" spans="2:7" ht="13">
+      <c r="B11" s="113" t="s">
         <v>258</v>
       </c>
-      <c r="C11" s="116">
+      <c r="C11" s="114">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="115" t="s">
+    <row r="12" spans="2:7" ht="13">
+      <c r="B12" s="113" t="s">
         <v>257</v>
       </c>
-      <c r="C12" s="116">
+      <c r="C12" s="114">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="115" t="s">
+    <row r="13" spans="2:7" ht="13">
+      <c r="B13" s="113" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="116">
+      <c r="C13" s="114">
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="115" t="s">
+    <row r="14" spans="2:7" ht="13">
+      <c r="B14" s="113" t="s">
         <v>255</v>
       </c>
-      <c r="C14" s="116">
+      <c r="C14" s="114">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
@@ -4320,13 +4333,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="119" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="117"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="117" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="115"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4351,10 +4364,10 @@
       <c r="G1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="118">
+      <c r="H1" s="116">
         <v>33344</v>
       </c>
-      <c r="I1" s="117">
+      <c r="I1" s="115">
         <v>11.25</v>
       </c>
     </row>
@@ -4380,10 +4393,10 @@
       <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="118">
+      <c r="H2" s="116">
         <v>29153</v>
       </c>
-      <c r="I2" s="117">
+      <c r="I2" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -4409,10 +4422,10 @@
       <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="118">
+      <c r="H3" s="116">
         <v>32040</v>
       </c>
-      <c r="I3" s="117">
+      <c r="I3" s="115">
         <v>14.55</v>
       </c>
     </row>
@@ -4438,10 +4451,10 @@
       <c r="G4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="118">
+      <c r="H4" s="116">
         <v>33823</v>
       </c>
-      <c r="I4" s="117">
+      <c r="I4" s="115">
         <v>11.25</v>
       </c>
     </row>
@@ -4467,10 +4480,10 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="118">
+      <c r="H5" s="116">
         <v>31503</v>
       </c>
-      <c r="I5" s="117">
+      <c r="I5" s="115">
         <v>10.199999999999999</v>
       </c>
     </row>
@@ -4496,10 +4509,10 @@
       <c r="G6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="118">
+      <c r="H6" s="116">
         <v>32894</v>
       </c>
-      <c r="I6" s="117">
+      <c r="I6" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -4525,10 +4538,10 @@
       <c r="G7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="118">
+      <c r="H7" s="116">
         <v>35886</v>
       </c>
-      <c r="I7" s="117">
+      <c r="I7" s="115">
         <v>9.9499999999999993</v>
       </c>
     </row>
@@ -4554,10 +4567,10 @@
       <c r="G8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="118">
+      <c r="H8" s="116">
         <v>31051</v>
       </c>
-      <c r="I8" s="117">
+      <c r="I8" s="115">
         <v>12.3</v>
       </c>
     </row>
@@ -4583,10 +4596,10 @@
       <c r="G9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="118">
+      <c r="H9" s="116">
         <v>31050</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="115">
         <v>13.25</v>
       </c>
     </row>
@@ -4612,10 +4625,10 @@
       <c r="G10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="118">
+      <c r="H10" s="116">
         <v>30939</v>
       </c>
-      <c r="I10" s="117">
+      <c r="I10" s="115">
         <v>10.199999999999999</v>
       </c>
     </row>
@@ -4641,10 +4654,10 @@
       <c r="G11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="118">
+      <c r="H11" s="116">
         <v>32863</v>
       </c>
-      <c r="I11" s="117">
+      <c r="I11" s="115">
         <v>12.2</v>
       </c>
     </row>
@@ -4670,10 +4683,10 @@
       <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="118">
+      <c r="H12" s="116">
         <v>30900</v>
       </c>
-      <c r="I12" s="117">
+      <c r="I12" s="115">
         <v>14.25</v>
       </c>
     </row>
@@ -4699,10 +4712,10 @@
       <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="118">
+      <c r="H13" s="116">
         <v>31689</v>
       </c>
-      <c r="I13" s="117">
+      <c r="I13" s="115">
         <v>11.5</v>
       </c>
     </row>
@@ -4728,10 +4741,10 @@
       <c r="G14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="118">
+      <c r="H14" s="116">
         <v>32561</v>
       </c>
-      <c r="I14" s="117">
+      <c r="I14" s="115">
         <v>10.35</v>
       </c>
     </row>
@@ -4757,10 +4770,10 @@
       <c r="G15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="118">
+      <c r="H15" s="116">
         <v>32979</v>
       </c>
-      <c r="I15" s="117">
+      <c r="I15" s="115">
         <v>10.15</v>
       </c>
     </row>
@@ -4786,10 +4799,10 @@
       <c r="G16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="118">
+      <c r="H16" s="116">
         <v>30386</v>
       </c>
-      <c r="I16" s="117">
+      <c r="I16" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -4815,10 +4828,10 @@
       <c r="G17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="118">
+      <c r="H17" s="116">
         <v>31217</v>
       </c>
-      <c r="I17" s="117">
+      <c r="I17" s="115">
         <v>13.25</v>
       </c>
     </row>
@@ -4844,10 +4857,10 @@
       <c r="G18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="118">
+      <c r="H18" s="116">
         <v>31112</v>
       </c>
-      <c r="I18" s="117">
+      <c r="I18" s="115">
         <v>9.5</v>
       </c>
     </row>
@@ -4873,10 +4886,10 @@
       <c r="G19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="118">
+      <c r="H19" s="116">
         <v>31805</v>
       </c>
-      <c r="I19" s="117">
+      <c r="I19" s="115">
         <v>11.3</v>
       </c>
     </row>
@@ -4902,10 +4915,10 @@
       <c r="G20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="118">
+      <c r="H20" s="116">
         <v>32125</v>
       </c>
-      <c r="I20" s="117">
+      <c r="I20" s="115">
         <v>12.35</v>
       </c>
     </row>
@@ -4931,10 +4944,10 @@
       <c r="G21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="118">
+      <c r="H21" s="116">
         <v>32979</v>
       </c>
-      <c r="I21" s="117">
+      <c r="I21" s="115">
         <v>11.9</v>
       </c>
     </row>
@@ -4960,10 +4973,10 @@
       <c r="G22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="118">
+      <c r="H22" s="116">
         <v>33688</v>
       </c>
-      <c r="I22" s="117">
+      <c r="I22" s="115">
         <v>11.85</v>
       </c>
     </row>
@@ -4989,10 +5002,10 @@
       <c r="G23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="118">
+      <c r="H23" s="116">
         <v>29885</v>
       </c>
-      <c r="I23" s="117">
+      <c r="I23" s="115">
         <v>10.75</v>
       </c>
     </row>
@@ -5018,10 +5031,10 @@
       <c r="G24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="118">
+      <c r="H24" s="116">
         <v>33091</v>
       </c>
-      <c r="I24" s="117">
+      <c r="I24" s="115">
         <v>9.75</v>
       </c>
     </row>
@@ -5047,10 +5060,10 @@
       <c r="G25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="118">
+      <c r="H25" s="116">
         <v>28531</v>
       </c>
-      <c r="I25" s="117">
+      <c r="I25" s="115">
         <v>13.95</v>
       </c>
     </row>
@@ -5076,10 +5089,10 @@
       <c r="G26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="118">
+      <c r="H26" s="116">
         <v>30028</v>
       </c>
-      <c r="I26" s="117">
+      <c r="I26" s="115">
         <v>11.2</v>
       </c>
     </row>
@@ -5105,10 +5118,10 @@
       <c r="G27" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="118">
+      <c r="H27" s="116">
         <v>33231</v>
       </c>
-      <c r="I27" s="117">
+      <c r="I27" s="115">
         <v>10.3</v>
       </c>
     </row>
@@ -5134,10 +5147,10 @@
       <c r="G28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="118">
+      <c r="H28" s="116">
         <v>32571</v>
       </c>
-      <c r="I28" s="117">
+      <c r="I28" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -5163,10 +5176,10 @@
       <c r="G29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="118">
+      <c r="H29" s="116">
         <v>30817</v>
       </c>
-      <c r="I29" s="117">
+      <c r="I29" s="115">
         <v>10.25</v>
       </c>
     </row>
@@ -5192,10 +5205,10 @@
       <c r="G30" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="118">
+      <c r="H30" s="116">
         <v>32679</v>
       </c>
-      <c r="I30" s="117">
+      <c r="I30" s="115">
         <v>9.85</v>
       </c>
     </row>
@@ -5221,10 +5234,10 @@
       <c r="G31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H31" s="118">
+      <c r="H31" s="116">
         <v>31729</v>
       </c>
-      <c r="I31" s="117">
+      <c r="I31" s="115">
         <v>11.65</v>
       </c>
     </row>
@@ -5250,10 +5263,10 @@
       <c r="G32" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="118">
+      <c r="H32" s="116">
         <v>33559</v>
       </c>
-      <c r="I32" s="117">
+      <c r="I32" s="115">
         <v>9.25</v>
       </c>
     </row>
@@ -5279,10 +5292,10 @@
       <c r="G33" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="118">
+      <c r="H33" s="116">
         <v>35125</v>
       </c>
-      <c r="I33" s="117">
+      <c r="I33" s="115">
         <v>9.25</v>
       </c>
     </row>
@@ -5308,10 +5321,10 @@
       <c r="G34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="118">
+      <c r="H34" s="116">
         <v>35609</v>
       </c>
-      <c r="I34" s="117">
+      <c r="I34" s="115">
         <v>11</v>
       </c>
     </row>
@@ -5337,10 +5350,10 @@
       <c r="G35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H35" s="118">
+      <c r="H35" s="116">
         <v>35840</v>
       </c>
-      <c r="I35" s="117">
+      <c r="I35" s="115">
         <v>10.95</v>
       </c>
     </row>
@@ -5366,10 +5379,10 @@
       <c r="G36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="118">
+      <c r="H36" s="116">
         <v>35855</v>
       </c>
-      <c r="I36" s="117">
+      <c r="I36" s="115">
         <v>11.75</v>
       </c>
     </row>
@@ -5395,10 +5408,10 @@
       <c r="G37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="118">
+      <c r="H37" s="116">
         <v>35981</v>
       </c>
-      <c r="I37" s="117">
+      <c r="I37" s="115">
         <v>10.15</v>
       </c>
     </row>
@@ -5416,20 +5429,20 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="18"/>
-    <col min="7" max="7" width="13.7109375" style="18" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="18"/>
+    <col min="4" max="4" width="12.54296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="18"/>
+    <col min="7" max="7" width="13.7265625" style="18" customWidth="1"/>
+    <col min="8" max="9" width="12.7265625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="15.5">
       <c r="A2" s="29" t="s">
         <v>143</v>
       </c>
@@ -5455,7 +5468,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75">
+    <row r="3" spans="1:9" ht="15.5">
       <c r="A3" s="19" t="s">
         <v>145</v>
       </c>
@@ -5478,7 +5491,7 @@
       <c r="H3" s="26"/>
       <c r="I3" s="27"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="13">
       <c r="A4" s="19" t="s">
         <v>145</v>
       </c>
@@ -5505,7 +5518,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75">
+    <row r="5" spans="1:9" ht="15.5">
       <c r="A5" s="19" t="s">
         <v>145</v>
       </c>
@@ -10349,13 +10362,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="119" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="117"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="117" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="115"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -10380,10 +10393,10 @@
       <c r="G1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="118">
+      <c r="H1" s="116">
         <v>33344</v>
       </c>
-      <c r="I1" s="117">
+      <c r="I1" s="115">
         <v>11.25</v>
       </c>
     </row>
@@ -10409,10 +10422,10 @@
       <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="118">
+      <c r="H2" s="116">
         <v>29153</v>
       </c>
-      <c r="I2" s="117">
+      <c r="I2" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -10438,10 +10451,10 @@
       <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="118">
+      <c r="H3" s="116">
         <v>32040</v>
       </c>
-      <c r="I3" s="117">
+      <c r="I3" s="115">
         <v>14.55</v>
       </c>
     </row>
@@ -10467,10 +10480,10 @@
       <c r="G4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="118">
+      <c r="H4" s="116">
         <v>33823</v>
       </c>
-      <c r="I4" s="117">
+      <c r="I4" s="115">
         <v>11.25</v>
       </c>
     </row>
@@ -10496,10 +10509,10 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="118">
+      <c r="H5" s="116">
         <v>31503</v>
       </c>
-      <c r="I5" s="117">
+      <c r="I5" s="115">
         <v>10.199999999999999</v>
       </c>
     </row>
@@ -10525,10 +10538,10 @@
       <c r="G6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="118">
+      <c r="H6" s="116">
         <v>32894</v>
       </c>
-      <c r="I6" s="117">
+      <c r="I6" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -10554,10 +10567,10 @@
       <c r="G7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="118">
+      <c r="H7" s="116">
         <v>35886</v>
       </c>
-      <c r="I7" s="117">
+      <c r="I7" s="115">
         <v>9.9499999999999993</v>
       </c>
     </row>
@@ -10583,10 +10596,10 @@
       <c r="G8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="118">
+      <c r="H8" s="116">
         <v>31051</v>
       </c>
-      <c r="I8" s="117">
+      <c r="I8" s="115">
         <v>12.3</v>
       </c>
     </row>
@@ -10612,10 +10625,10 @@
       <c r="G9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="118">
+      <c r="H9" s="116">
         <v>31050</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="115">
         <v>13.25</v>
       </c>
     </row>
@@ -10641,10 +10654,10 @@
       <c r="G10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="118">
+      <c r="H10" s="116">
         <v>30939</v>
       </c>
-      <c r="I10" s="117">
+      <c r="I10" s="115">
         <v>10.199999999999999</v>
       </c>
     </row>
@@ -10670,10 +10683,10 @@
       <c r="G11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="118">
+      <c r="H11" s="116">
         <v>32863</v>
       </c>
-      <c r="I11" s="117">
+      <c r="I11" s="115">
         <v>12.2</v>
       </c>
     </row>
@@ -10699,10 +10712,10 @@
       <c r="G12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="118">
+      <c r="H12" s="116">
         <v>30900</v>
       </c>
-      <c r="I12" s="117">
+      <c r="I12" s="115">
         <v>14.25</v>
       </c>
     </row>
@@ -10728,10 +10741,10 @@
       <c r="G13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="118">
+      <c r="H13" s="116">
         <v>31689</v>
       </c>
-      <c r="I13" s="117">
+      <c r="I13" s="115">
         <v>11.5</v>
       </c>
     </row>
@@ -10757,10 +10770,10 @@
       <c r="G14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="118">
+      <c r="H14" s="116">
         <v>32561</v>
       </c>
-      <c r="I14" s="117">
+      <c r="I14" s="115">
         <v>10.35</v>
       </c>
     </row>
@@ -10786,10 +10799,10 @@
       <c r="G15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="118">
+      <c r="H15" s="116">
         <v>32979</v>
       </c>
-      <c r="I15" s="117">
+      <c r="I15" s="115">
         <v>10.15</v>
       </c>
     </row>
@@ -10815,10 +10828,10 @@
       <c r="G16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="118">
+      <c r="H16" s="116">
         <v>30386</v>
       </c>
-      <c r="I16" s="117">
+      <c r="I16" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -10844,10 +10857,10 @@
       <c r="G17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="118">
+      <c r="H17" s="116">
         <v>31217</v>
       </c>
-      <c r="I17" s="117">
+      <c r="I17" s="115">
         <v>13.25</v>
       </c>
     </row>
@@ -10873,10 +10886,10 @@
       <c r="G18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="118">
+      <c r="H18" s="116">
         <v>31112</v>
       </c>
-      <c r="I18" s="117">
+      <c r="I18" s="115">
         <v>9.5</v>
       </c>
     </row>
@@ -10902,10 +10915,10 @@
       <c r="G19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="118">
+      <c r="H19" s="116">
         <v>31805</v>
       </c>
-      <c r="I19" s="117">
+      <c r="I19" s="115">
         <v>11.3</v>
       </c>
     </row>
@@ -10931,10 +10944,10 @@
       <c r="G20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="118">
+      <c r="H20" s="116">
         <v>32125</v>
       </c>
-      <c r="I20" s="117">
+      <c r="I20" s="115">
         <v>12.35</v>
       </c>
     </row>
@@ -10960,10 +10973,10 @@
       <c r="G21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="118">
+      <c r="H21" s="116">
         <v>32979</v>
       </c>
-      <c r="I21" s="117">
+      <c r="I21" s="115">
         <v>11.9</v>
       </c>
     </row>
@@ -10989,10 +11002,10 @@
       <c r="G22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="118">
+      <c r="H22" s="116">
         <v>33688</v>
       </c>
-      <c r="I22" s="117">
+      <c r="I22" s="115">
         <v>11.85</v>
       </c>
     </row>
@@ -11018,10 +11031,10 @@
       <c r="G23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="118">
+      <c r="H23" s="116">
         <v>29885</v>
       </c>
-      <c r="I23" s="117">
+      <c r="I23" s="115">
         <v>10.75</v>
       </c>
     </row>
@@ -11047,10 +11060,10 @@
       <c r="G24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="118">
+      <c r="H24" s="116">
         <v>33091</v>
       </c>
-      <c r="I24" s="117">
+      <c r="I24" s="115">
         <v>9.75</v>
       </c>
     </row>
@@ -11076,10 +11089,10 @@
       <c r="G25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H25" s="118">
+      <c r="H25" s="116">
         <v>28531</v>
       </c>
-      <c r="I25" s="117">
+      <c r="I25" s="115">
         <v>13.95</v>
       </c>
     </row>
@@ -11105,10 +11118,10 @@
       <c r="G26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="118">
+      <c r="H26" s="116">
         <v>30028</v>
       </c>
-      <c r="I26" s="117">
+      <c r="I26" s="115">
         <v>11.2</v>
       </c>
     </row>
@@ -11134,10 +11147,10 @@
       <c r="G27" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="118">
+      <c r="H27" s="116">
         <v>33231</v>
       </c>
-      <c r="I27" s="117">
+      <c r="I27" s="115">
         <v>10.3</v>
       </c>
     </row>
@@ -11163,10 +11176,10 @@
       <c r="G28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="118">
+      <c r="H28" s="116">
         <v>32571</v>
       </c>
-      <c r="I28" s="117">
+      <c r="I28" s="115">
         <v>12.25</v>
       </c>
     </row>
@@ -11192,10 +11205,10 @@
       <c r="G29" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="118">
+      <c r="H29" s="116">
         <v>30817</v>
       </c>
-      <c r="I29" s="117">
+      <c r="I29" s="115">
         <v>10.25</v>
       </c>
     </row>
@@ -11221,10 +11234,10 @@
       <c r="G30" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="118">
+      <c r="H30" s="116">
         <v>32679</v>
       </c>
-      <c r="I30" s="117">
+      <c r="I30" s="115">
         <v>9.85</v>
       </c>
     </row>
@@ -11250,10 +11263,10 @@
       <c r="G31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H31" s="118">
+      <c r="H31" s="116">
         <v>31729</v>
       </c>
-      <c r="I31" s="117">
+      <c r="I31" s="115">
         <v>11.65</v>
       </c>
     </row>
@@ -11279,10 +11292,10 @@
       <c r="G32" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="118">
+      <c r="H32" s="116">
         <v>33559</v>
       </c>
-      <c r="I32" s="117">
+      <c r="I32" s="115">
         <v>9.25</v>
       </c>
     </row>
@@ -11308,10 +11321,10 @@
       <c r="G33" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="118">
+      <c r="H33" s="116">
         <v>35125</v>
       </c>
-      <c r="I33" s="117">
+      <c r="I33" s="115">
         <v>9.25</v>
       </c>
     </row>
@@ -11337,10 +11350,10 @@
       <c r="G34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H34" s="118">
+      <c r="H34" s="116">
         <v>35609</v>
       </c>
-      <c r="I34" s="117">
+      <c r="I34" s="115">
         <v>11</v>
       </c>
     </row>
@@ -11366,10 +11379,10 @@
       <c r="G35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H35" s="118">
+      <c r="H35" s="116">
         <v>35840</v>
       </c>
-      <c r="I35" s="117">
+      <c r="I35" s="115">
         <v>10.95</v>
       </c>
     </row>
@@ -11395,10 +11408,10 @@
       <c r="G36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="118">
+      <c r="H36" s="116">
         <v>35855</v>
       </c>
-      <c r="I36" s="117">
+      <c r="I36" s="115">
         <v>11.75</v>
       </c>
     </row>
@@ -11424,10 +11437,10 @@
       <c r="G37" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="118">
+      <c r="H37" s="116">
         <v>35981</v>
       </c>
-      <c r="I37" s="117">
+      <c r="I37" s="115">
         <v>10.15</v>
       </c>
     </row>
@@ -11445,16 +11458,16 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" customWidth="1"/>
+    <col min="2" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="6" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="3.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="13.5" thickBot="1"/>
+    <row r="1" spans="2:7" ht="13" thickBot="1"/>
     <row r="2" spans="2:7" ht="21.75" customHeight="1">
       <c r="B2" s="33" t="s">
         <v>16</v>
@@ -11471,7 +11484,7 @@
       <c r="F2" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="125"/>
+      <c r="G2" s="123"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="10">
@@ -11484,7 +11497,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="G3" s="68"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="10">
@@ -11497,7 +11510,7 @@
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
-      <c r="G4" s="68"/>
+      <c r="G4" s="66"/>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="10">
@@ -11510,7 +11523,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="68"/>
+      <c r="G5" s="66"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="10">
@@ -11523,7 +11536,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="68"/>
+      <c r="G6" s="66"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="10">
@@ -11536,7 +11549,7 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="68"/>
+      <c r="G7" s="66"/>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="10">
@@ -11549,7 +11562,7 @@
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="68"/>
+      <c r="G8" s="66"/>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="10">
@@ -11562,7 +11575,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="68"/>
+      <c r="G9" s="66"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="10">
@@ -11575,7 +11588,7 @@
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="68"/>
+      <c r="G10" s="66"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="10"/>
@@ -11586,7 +11599,7 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="68"/>
+      <c r="G11" s="66"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="10"/>
@@ -11597,7 +11610,7 @@
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="68"/>
+      <c r="G12" s="66"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="10"/>
@@ -11608,7 +11621,7 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="68"/>
+      <c r="G13" s="66"/>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="10">
@@ -11621,7 +11634,7 @@
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="68"/>
+      <c r="G14" s="66"/>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="10">
@@ -11634,7 +11647,7 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="68"/>
+      <c r="G15" s="66"/>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="10">
@@ -11647,7 +11660,7 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="68"/>
+      <c r="G16" s="66"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="10">
@@ -11660,9 +11673,9 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="68"/>
-    </row>
-    <row r="18" spans="2:7" ht="13.5" thickBot="1">
+      <c r="G17" s="66"/>
+    </row>
+    <row r="18" spans="2:7" ht="13" thickBot="1">
       <c r="B18" s="13">
         <v>1368</v>
       </c>
@@ -11673,7 +11686,7 @@
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="68"/>
+      <c r="G18" s="66"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -11692,8 +11705,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="8" width="14.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="1" max="8" width="14.1796875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" customHeight="1">
@@ -12814,57 +12827,57 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="56" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="56" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="56" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="56" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="30.1796875" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" style="54" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="54" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="7.26953125" style="54" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" style="54" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" style="54" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" thickBot="1"/>
+    <row r="1" spans="1:2" ht="13" thickBot="1"/>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="128" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="131"/>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" thickTop="1" thickBot="1">
-      <c r="A3" s="62" t="s">
+      <c r="B2" s="129"/>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A3" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="59" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="7.5" customHeight="1" thickTop="1">
-      <c r="A4" s="60"/>
-      <c r="B4" s="59"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="63" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="57"/>
+    </row>
+    <row r="5" spans="1:2" ht="13">
+      <c r="A5" s="61" t="s">
         <v>229</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="56">
         <f>HLOOKUP($B$3,'Master Inventory List'!$A$2:$G$5,2,FALSE)</f>
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="63" t="s">
+    <row r="6" spans="1:2" ht="13">
+      <c r="A6" s="61" t="s">
         <v>228</v>
       </c>
-      <c r="B6" s="58"/>
+      <c r="B6" s="56"/>
     </row>
     <row r="7" spans="1:2" ht="13.5" thickBot="1">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="58"/>
+      <c r="B7" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12884,101 +12897,101 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="56" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="14.81640625" style="54" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="54"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
-      <c r="A2" s="65" t="s">
+    <row r="2" spans="1:7" ht="13">
+      <c r="A2" s="63" t="s">
         <v>238</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="64" t="s">
         <v>237</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="64" t="s">
         <v>235</v>
       </c>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="64" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="67" t="s">
+    <row r="3" spans="1:7" ht="13">
+      <c r="A3" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="B3" s="57">
+      <c r="B3" s="55">
         <v>120</v>
       </c>
-      <c r="C3" s="57">
+      <c r="C3" s="55">
         <v>150</v>
       </c>
-      <c r="D3" s="57">
+      <c r="D3" s="55">
         <v>135</v>
       </c>
-      <c r="E3" s="57">
+      <c r="E3" s="55">
         <v>90</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="55">
         <v>95</v>
       </c>
-      <c r="G3" s="57">
+      <c r="G3" s="55">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="67" t="s">
+    <row r="4" spans="1:7" ht="13">
+      <c r="A4" s="65" t="s">
         <v>233</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="55">
         <v>55</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="55">
         <v>110</v>
       </c>
-      <c r="D4" s="57">
+      <c r="D4" s="55">
         <v>75</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="55">
         <v>95</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="55">
         <v>75</v>
       </c>
-      <c r="G4" s="57">
+      <c r="G4" s="55">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:7" ht="13">
+      <c r="A5" s="65" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="57">
+      <c r="B5" s="55">
         <v>70</v>
       </c>
-      <c r="C5" s="57">
+      <c r="C5" s="55">
         <v>115</v>
       </c>
-      <c r="D5" s="57">
+      <c r="D5" s="55">
         <v>65</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="55">
         <v>55</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="55">
         <v>85</v>
       </c>
-      <c r="G5" s="57">
+      <c r="G5" s="55">
         <v>65</v>
       </c>
     </row>
@@ -12996,135 +13009,135 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1796875" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="41.25" customHeight="1" thickBot="1">
-      <c r="C2" s="121" t="s">
+      <c r="C2" s="119" t="s">
         <v>281</v>
       </c>
-      <c r="D2" s="124" t="s">
+      <c r="D2" s="122" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15">
-      <c r="B3" s="120" t="s">
+    <row r="3" spans="2:6" ht="14">
+      <c r="B3" s="118" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="120" t="s">
         <v>240</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="F3" s="123" t="s">
+      <c r="F3" s="121" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="69">
+      <c r="B4" s="67">
         <v>1054</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="F4" s="70"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="F4" s="68"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="69">
+      <c r="B5" s="67">
         <v>1078</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="F5" s="70"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="F5" s="68"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="69">
+      <c r="B6" s="67">
         <v>1284</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="F6" s="70"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="F6" s="68"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="69">
+      <c r="B7" s="67">
         <v>1299</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="F7" s="68"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="69">
+      <c r="B8" s="67">
         <v>1329</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="F8" s="70"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="F8" s="68"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="69">
+      <c r="B9" s="67">
         <v>1509</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="F9" s="68"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="F10" s="70"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="F11" s="70"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="F11" s="68"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="F12" s="70"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="F12" s="68"/>
     </row>
     <row r="13" spans="2:6">
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="F13" s="70"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="F13" s="68"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="F14" s="70"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="F14" s="68"/>
     </row>
     <row r="15" spans="2:6">
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="F15" s="70"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="F15" s="68"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="F16" s="70"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="F16" s="68"/>
     </row>
     <row r="17" spans="3:6">
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="F17" s="70"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="F17" s="68"/>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="F18" s="70"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="F18" s="68"/>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="F19" s="70"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="F19" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13142,8 +13155,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1"/>
   <cols>
-    <col min="1" max="8" width="14.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="1" max="8" width="14.1796875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="24.75" customHeight="1">
@@ -14265,19 +14278,19 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="3.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="13">
       <c r="A2" s="35" t="s">
         <v>168</v>
       </c>
@@ -14301,7 +14314,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="13">
       <c r="A3" s="22" t="s">
         <v>169</v>
       </c>
@@ -14325,7 +14338,7 @@
         <v>WW</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="13">
       <c r="A4" s="22" t="s">
         <v>170</v>
       </c>
@@ -14340,7 +14353,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="13">
       <c r="A5" s="22" t="s">
         <v>171</v>
       </c>
@@ -14355,7 +14368,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="13">
       <c r="A6" s="22" t="s">
         <v>172</v>
       </c>
@@ -14370,7 +14383,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="13">
       <c r="A7" s="22" t="s">
         <v>173</v>
       </c>
@@ -14385,7 +14398,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="13">
       <c r="A8" s="22" t="s">
         <v>174</v>
       </c>
@@ -14400,7 +14413,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="13">
       <c r="A9" s="22" t="s">
         <v>175</v>
       </c>
@@ -14415,7 +14428,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="13">
       <c r="A10" s="22" t="s">
         <v>176</v>
       </c>
@@ -14430,7 +14443,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="13">
       <c r="A11" s="22" t="s">
         <v>177</v>
       </c>
@@ -14445,7 +14458,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="13">
       <c r="A12" s="22" t="s">
         <v>204</v>
       </c>
@@ -14460,7 +14473,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="13">
       <c r="A13" s="22" t="s">
         <v>205</v>
       </c>
@@ -14475,7 +14488,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="13">
       <c r="A14" s="22" t="s">
         <v>206</v>
       </c>
@@ -14490,7 +14503,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="13">
       <c r="A15" s="22" t="s">
         <v>207</v>
       </c>
@@ -14505,7 +14518,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="13">
       <c r="A16" s="22" t="s">
         <v>208</v>
       </c>
@@ -14520,7 +14533,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="13">
       <c r="A17" s="22" t="s">
         <v>209</v>
       </c>
@@ -14535,7 +14548,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="13">
       <c r="A18" s="22" t="s">
         <v>210</v>
       </c>
@@ -14550,7 +14563,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="13">
       <c r="A19" s="22" t="s">
         <v>178</v>
       </c>
@@ -14565,7 +14578,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="13">
       <c r="A20" s="22" t="s">
         <v>211</v>
       </c>
@@ -14580,7 +14593,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="13">
       <c r="A21" s="22" t="s">
         <v>212</v>
       </c>
@@ -14595,7 +14608,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="13">
       <c r="A22" s="22" t="s">
         <v>217</v>
       </c>
@@ -14610,7 +14623,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="13">
       <c r="A23" s="22" t="s">
         <v>218</v>
       </c>
@@ -14625,7 +14638,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="13">
       <c r="A24" s="22" t="s">
         <v>214</v>
       </c>
@@ -14640,7 +14653,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="13">
       <c r="A25" s="22" t="s">
         <v>215</v>
       </c>
@@ -14655,7 +14668,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="13">
       <c r="A26" s="22" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
Completed Advantages and Disadvantages of Excel Name Ranges
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1476" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBE5BD6F-5D84-4168-88D7-425BE394E8F1}"/>
+  <xr:revisionPtr revIDLastSave="1479" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0FD8CA4-0681-4282-9A0C-A88E691965B3}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,6 +98,7 @@
     <definedName name="solver_val" localSheetId="15" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="15" hidden="1">3</definedName>
+    <definedName name="Totals">'IF Function'!$F$5:$F$9</definedName>
     <definedName name="Week_1">'IF Function'!$B$5:$B$9</definedName>
     <definedName name="Week_2">'IF Function'!$C$5:$C$9</definedName>
     <definedName name="Week_3">'IF Function'!$D$5:$D$9</definedName>
@@ -1966,13 +1967,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2867,7 +2868,10 @@
         <f>SUM(Week_4)</f>
         <v>46624</v>
       </c>
-      <c r="F10" s="53"/>
+      <c r="F10" s="53">
+        <f>SUM(Totals)</f>
+        <v>176211</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="14">
       <c r="A11" s="49"/>
@@ -2976,10 +2980,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -2988,11 +2992,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3001,8 +3005,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3011,8 +3015,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3021,8 +3025,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3031,8 +3035,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3041,8 +3045,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3051,8 +3055,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3061,8 +3065,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3071,8 +3075,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3081,8 +3085,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3091,8 +3095,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3101,8 +3105,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3111,8 +3115,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3121,8 +3125,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3131,8 +3135,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3141,18 +3145,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3163,6 +3160,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Editing an Excel Name Range
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1479" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0FD8CA4-0681-4282-9A0C-A88E691965B3}"/>
+  <xr:revisionPtr revIDLastSave="1480" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2157988-3E20-470A-A735-E54AC1EF2246}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,8 +38,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
-    <definedName name="Gross_Margin">#REF!</definedName>
-    <definedName name="List">#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="15" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -1967,13 +1965,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2673,7 +2671,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2980,10 +2978,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -2992,11 +2990,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3005,8 +3003,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3015,8 +3013,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3025,8 +3023,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3035,8 +3033,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3045,8 +3043,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3055,8 +3053,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3065,8 +3063,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3075,8 +3073,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3085,8 +3083,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3095,8 +3093,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3105,8 +3103,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3115,8 +3113,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3125,8 +3123,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3135,8 +3133,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3145,11 +3143,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3160,13 +3165,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Using Excel's IF() Function
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1480" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2157988-3E20-470A-A735-E54AC1EF2246}"/>
+  <xr:revisionPtr revIDLastSave="1482" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2CF57B0-577C-464B-B8CF-3CE498944D34}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1965,13 +1965,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2671,7 +2671,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2751,7 +2751,10 @@
         <f>SUM(B5:E5)</f>
         <v>36245</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="str">
+        <f>IF(F5&gt;=$I$2,"YES","NO")</f>
+        <v>YES</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="15.5">
@@ -2978,10 +2981,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -2990,11 +2993,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3003,8 +3006,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3013,8 +3016,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3023,8 +3026,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3033,8 +3036,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3043,8 +3046,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3053,8 +3056,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3063,8 +3066,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3073,8 +3076,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3083,8 +3086,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3093,8 +3096,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3103,8 +3106,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3113,8 +3116,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3123,8 +3126,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3133,8 +3136,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3143,18 +3146,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3165,6 +3161,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Excel's IF() Function with a Name Range
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1482" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2CF57B0-577C-464B-B8CF-3CE498944D34}"/>
+  <xr:revisionPtr revIDLastSave="1485" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0260F2D5-CDBE-4880-B609-C382B35D47A2}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,6 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'INDEX MATCH Master Emp List'!$A$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
+    <definedName name="Monthly_Goal">'IF Function'!$I$2</definedName>
     <definedName name="solver_cvg" localSheetId="15" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -1965,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2671,7 +2672,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2752,7 +2753,7 @@
         <v>36245</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f>IF(F5&gt;=$I$2,"YES","NO")</f>
+        <f>IF(F5&gt;=Monthly_Goal,"YES","NO")</f>
         <v>YES</v>
       </c>
       <c r="I5" s="2"/>
@@ -2777,7 +2778,10 @@
         <f>SUM(B6:E6)</f>
         <v>31475</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="str">
+        <f>IF(F6&gt;=Monthly_Goal,"YES","NO")</f>
+        <v>NO</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15.5">
@@ -2800,7 +2804,10 @@
         <f>SUM(B7:E7)</f>
         <v>33427</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="str">
+        <f>IF(F7&gt;=Monthly_Goal,"YES","NO")</f>
+        <v>NO</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="15.5">
@@ -2823,7 +2830,10 @@
         <f>SUM(B8:E8)</f>
         <v>39705</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="str">
+        <f>IF(F8&gt;=Monthly_Goal,"YES","NO")</f>
+        <v>YES</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="16" thickBot="1">
@@ -2846,7 +2856,10 @@
         <f>SUM(B9:E9)</f>
         <v>35359</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="str">
+        <f>IF(F9&gt;=Monthly_Goal,"YES","NO")</f>
+        <v>YES</v>
+      </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="14">
@@ -2981,10 +2994,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -2993,11 +3006,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3006,8 +3019,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3016,8 +3029,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3026,8 +3039,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3036,8 +3049,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3046,8 +3059,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3056,8 +3069,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3066,8 +3079,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3076,8 +3089,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3086,8 +3099,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3096,8 +3109,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3106,8 +3119,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3116,8 +3129,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3126,8 +3139,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3136,8 +3149,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3146,11 +3159,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3161,13 +3181,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Nesting Functions with Excel
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1485" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0260F2D5-CDBE-4880-B609-C382B35D47A2}"/>
+  <xr:revisionPtr revIDLastSave="1486" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE26A507-B9F2-4FBC-A8AC-00125BA802C9}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2672,7 +2672,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2756,7 +2756,10 @@
         <f>IF(F5&gt;=Monthly_Goal,"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="b">
+        <f>AND(H5="YES",MIN(B5:E5)&gt;=8000)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15.5">
       <c r="A6" s="5" t="s">
@@ -2994,10 +2997,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3006,11 +3009,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3019,8 +3022,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3029,8 +3032,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3039,8 +3042,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3049,8 +3052,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3059,8 +3062,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3069,8 +3072,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3079,8 +3082,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3089,8 +3092,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3099,8 +3102,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3109,8 +3112,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3119,8 +3122,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3129,8 +3132,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3139,8 +3142,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3149,8 +3152,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3159,18 +3162,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3181,6 +3177,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Nesting Excels AND() Function within the IF() Function
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1486" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE26A507-B9F2-4FBC-A8AC-00125BA802C9}"/>
+  <xr:revisionPtr revIDLastSave="1488" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBEBFF15-0AA0-4F9B-B9EA-2718D6E5FF4B}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2672,7 +2672,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2756,9 +2756,9 @@
         <f>IF(F5&gt;=Monthly_Goal,"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="I5" s="2" t="b">
-        <f>AND(H5="YES",MIN(B5:E5)&gt;=8000)</f>
-        <v>1</v>
+      <c r="I5" s="2" t="str">
+        <f>IF(AND(H5="YES",MIN(B5:E5)&gt;=8000),"YES","NO")</f>
+        <v>YES</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.5">
@@ -2785,7 +2785,10 @@
         <f>IF(F6&gt;=Monthly_Goal,"YES","NO")</f>
         <v>NO</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="str">
+        <f t="shared" ref="I6:I9" si="0">IF(AND(H6="YES",MIN(B6:E6)&gt;=8000),"YES","NO")</f>
+        <v>NO</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15.5">
       <c r="A7" s="5" t="s">
@@ -2811,7 +2814,10 @@
         <f>IF(F7&gt;=Monthly_Goal,"YES","NO")</f>
         <v>NO</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15.5">
       <c r="A8" s="5" t="s">
@@ -2837,7 +2843,10 @@
         <f>IF(F8&gt;=Monthly_Goal,"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>YES</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="16" thickBot="1">
       <c r="A9" s="16" t="s">
@@ -2863,7 +2872,10 @@
         <f>IF(F9&gt;=Monthly_Goal,"YES","NO")</f>
         <v>YES</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>NO</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="14">
       <c r="A10" s="48" t="s">
@@ -2997,10 +3009,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3009,11 +3021,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3022,8 +3034,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3032,8 +3044,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3042,8 +3054,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3052,8 +3064,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3062,8 +3074,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3072,8 +3084,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3082,8 +3094,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3092,8 +3104,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3102,8 +3114,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3112,8 +3124,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3122,8 +3134,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3132,8 +3144,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3142,8 +3154,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3152,8 +3164,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3162,11 +3174,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3177,13 +3196,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Using Excel's COUNTIF() Function
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1488" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBEBFF15-0AA0-4F9B-B9EA-2718D6E5FF4B}"/>
+  <xr:revisionPtr revIDLastSave="1489" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C32D5BB-193A-4015-86DE-7977E1E2FA5D}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2672,7 +2672,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2913,7 +2913,10 @@
       <c r="C12" s="125"/>
       <c r="D12" s="125"/>
       <c r="E12" s="126"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <f>COUNTIF(H5:H9,"YES")</f>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3009,10 +3012,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3021,11 +3024,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3034,8 +3037,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3044,8 +3047,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3054,8 +3057,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3064,8 +3067,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3074,8 +3077,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3084,8 +3087,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3094,8 +3097,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3104,8 +3107,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3114,8 +3117,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3124,8 +3127,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3134,8 +3137,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3144,8 +3147,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3154,8 +3157,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3164,8 +3167,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3174,18 +3177,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3196,6 +3192,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Using Excel's SUMIF() Function
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1489" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C32D5BB-193A-4015-86DE-7977E1E2FA5D}"/>
+  <xr:revisionPtr revIDLastSave="1494" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD0B90FF-ED0A-4ED9-B73F-B0164B11CC2D}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2671,7 +2671,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3012,10 +3012,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3024,11 +3024,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3037,8 +3037,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3047,8 +3047,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3057,8 +3057,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3067,8 +3067,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3077,8 +3077,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3087,8 +3087,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3097,8 +3097,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130"/>
-      <c r="F10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3107,8 +3107,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130"/>
-      <c r="F11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3117,8 +3117,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3127,8 +3127,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130"/>
-      <c r="F13" s="131"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3137,8 +3137,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3147,8 +3147,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3157,8 +3157,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130"/>
-      <c r="F16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3167,8 +3167,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130"/>
-      <c r="F17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3177,11 +3177,18 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130"/>
-      <c r="F18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3192,13 +3199,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5461,8 +5461,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A2:I272"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -5524,8 +5524,14 @@
       <c r="G3" s="21">
         <v>3000</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="H3" s="26">
+        <f>SUMIF(B3:B272,G3,E3:E272)</f>
+        <v>17538</v>
+      </c>
+      <c r="I3" s="27">
+        <f>SUMIF(B3:B272,G3,D3:D272)</f>
+        <v>491064</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="13">
       <c r="A4" s="19" t="s">
@@ -5574,8 +5580,14 @@
       <c r="G5" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
+      <c r="H5" s="26">
+        <f>SUMIF(C3:C272,G5,E3:E272)</f>
+        <v>7357</v>
+      </c>
+      <c r="I5" s="27">
+        <f>SUMIF(C3:C272,G5,D3:D272)</f>
+        <v>205996</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="19" t="s">

</xml_diff>

<commit_message>
Completed Using Excel's IFERROR() Function
</commit_message>
<xml_diff>
--- a/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
+++ b/24 - Excels Conditional Functions/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/24 - Excels Conditional Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1494" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD0B90FF-ED0A-4ED9-B73F-B0164B11CC2D}"/>
+  <xr:revisionPtr revIDLastSave="1497" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49228E70-6A07-4051-941B-2CC0AFA56112}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1966,13 +1966,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3012,10 +3012,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="132" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="130"/>
+      <c r="F2" s="132"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -3024,11 +3024,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="131" t="str">
+      <c r="E3" s="130" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="132"/>
+      <c r="F3" s="131"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -3037,8 +3037,8 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="132"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="131"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -3047,8 +3047,8 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="131"/>
-      <c r="F5" s="132"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="131"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -3057,8 +3057,8 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="131"/>
-      <c r="F6" s="132"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="131"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -3067,8 +3067,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="131"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -3077,8 +3077,8 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="131"/>
-      <c r="F8" s="132"/>
+      <c r="E8" s="130"/>
+      <c r="F8" s="131"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -3087,8 +3087,8 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
+      <c r="E9" s="130"/>
+      <c r="F9" s="131"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -3097,8 +3097,8 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="131"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -3107,8 +3107,8 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -3117,8 +3117,8 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="131"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -3127,8 +3127,8 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="131"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -3137,8 +3137,8 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -3147,8 +3147,8 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="132"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="131"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -3157,8 +3157,8 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="131"/>
-      <c r="F16" s="132"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -3167,8 +3167,8 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="131"/>
-      <c r="F17" s="132"/>
+      <c r="E17" s="130"/>
+      <c r="F17" s="131"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -3177,18 +3177,11 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="131"/>
-      <c r="F18" s="132"/>
+      <c r="E18" s="130"/>
+      <c r="F18" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3199,6 +3192,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5461,7 +5461,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A2:I272"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -11502,14 +11502,15 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
     <col min="1" max="1" width="3.453125" customWidth="1"/>
-    <col min="2" max="3" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="5" max="6" width="13.81640625" customWidth="1"/>
     <col min="7" max="7" width="3.1796875" customWidth="1"/>
@@ -11539,7 +11540,7 @@
         <v>1054</v>
       </c>
       <c r="C3" s="11" t="str">
-        <f>VLOOKUP($B3,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B3,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Howard</v>
       </c>
       <c r="D3" s="11"/>
@@ -11552,7 +11553,7 @@
         <v>1056</v>
       </c>
       <c r="C4" s="11" t="str">
-        <f>VLOOKUP($B4,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B4,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Joe</v>
       </c>
       <c r="D4" s="11"/>
@@ -11565,7 +11566,7 @@
         <v>1067</v>
       </c>
       <c r="C5" s="11" t="str">
-        <f>VLOOKUP($B5,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B5,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Gail</v>
       </c>
       <c r="D5" s="11"/>
@@ -11578,7 +11579,7 @@
         <v>1075</v>
       </c>
       <c r="C6" s="11" t="str">
-        <f>VLOOKUP($B6,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B6,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Sheryl</v>
       </c>
       <c r="D6" s="11"/>
@@ -11591,7 +11592,7 @@
         <v>1078</v>
       </c>
       <c r="C7" s="11" t="str">
-        <f>VLOOKUP($B7,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B7,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Kendrick</v>
       </c>
       <c r="D7" s="11"/>
@@ -11604,7 +11605,7 @@
         <v>1152</v>
       </c>
       <c r="C8" s="11" t="str">
-        <f>VLOOKUP($B8,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B8,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Mark</v>
       </c>
       <c r="D8" s="11"/>
@@ -11617,7 +11618,7 @@
         <v>1196</v>
       </c>
       <c r="C9" s="11" t="str">
-        <f>VLOOKUP($B9,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B9,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Katie</v>
       </c>
       <c r="D9" s="11"/>
@@ -11630,7 +11631,7 @@
         <v>1284</v>
       </c>
       <c r="C10" s="11" t="str">
-        <f>VLOOKUP($B10,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B10,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Frank</v>
       </c>
       <c r="D10" s="11"/>
@@ -11640,9 +11641,9 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="10"/>
-      <c r="C11" s="11" t="e">
-        <f>VLOOKUP($B11,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
-        <v>#N/A</v>
+      <c r="C11" s="11" t="str">
+        <f>IFERROR(VLOOKUP($B11,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
+        <v>EMP ID NOT FOUND</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -11651,9 +11652,9 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="10"/>
-      <c r="C12" s="11" t="e">
-        <f>VLOOKUP($B12,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
-        <v>#N/A</v>
+      <c r="C12" s="11" t="str">
+        <f>IFERROR(VLOOKUP($B12,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
+        <v>EMP ID NOT FOUND</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -11662,9 +11663,9 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="10"/>
-      <c r="C13" s="11" t="e">
-        <f>VLOOKUP($B13,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
-        <v>#N/A</v>
+      <c r="C13" s="11" t="str">
+        <f>IFERROR(VLOOKUP($B13,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
+        <v>EMP ID NOT FOUND</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -11676,7 +11677,7 @@
         <v>1302</v>
       </c>
       <c r="C14" s="11" t="str">
-        <f>VLOOKUP($B14,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B14,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Randy</v>
       </c>
       <c r="D14" s="11"/>
@@ -11689,7 +11690,7 @@
         <v>1310</v>
       </c>
       <c r="C15" s="11" t="str">
-        <f>VLOOKUP($B15,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B15,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Ellen</v>
       </c>
       <c r="D15" s="11"/>
@@ -11702,7 +11703,7 @@
         <v>1329</v>
       </c>
       <c r="C16" s="11" t="str">
-        <f>VLOOKUP($B16,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B16,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Tuome</v>
       </c>
       <c r="D16" s="11"/>
@@ -11715,7 +11716,7 @@
         <v>1333</v>
       </c>
       <c r="C17" s="11" t="str">
-        <f>VLOOKUP($B17,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B17,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Tadeuz</v>
       </c>
       <c r="D17" s="11"/>
@@ -11728,7 +11729,7 @@
         <v>1368</v>
       </c>
       <c r="C18" s="11" t="str">
-        <f>VLOOKUP($B18,'Master Emp List'!$A$1:$I$38,3,FALSE)</f>
+        <f>IFERROR(VLOOKUP($B18,'Master Emp List'!$A$1:$I$38,3,FALSE),"EMP ID NOT FOUND")</f>
         <v>Tammy</v>
       </c>
       <c r="D18" s="11"/>

</xml_diff>